<commit_message>
error in yields, check
</commit_message>
<xml_diff>
--- a/case study propionate/results_All_substrates.xlsx
+++ b/case study propionate/results_All_substrates.xlsx
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>182.7889166722919</v>
+        <v>148.0704815313893</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>444.9057959249311</v>
+        <v>444.9057959162892</v>
       </c>
     </row>
     <row r="16">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>130.8224491787346</v>
+        <v>130.8224491787308</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>9.079710120916967</v>
+        <v>9.079710120740593</v>
       </c>
     </row>
     <row r="19">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4.046055129239208</v>
+        <v>4.046055129239088</v>
       </c>
     </row>
     <row r="21">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>453.9855060458481</v>
+        <v>453.9855060370296</v>
       </c>
     </row>
     <row r="23">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>134.8685043079738</v>
+        <v>134.8685043079699</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>301463.2965074213</v>
+        <v>301463.2965074124</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>6069.082693858822</v>
+        <v>6069.082693858644</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>34065.35250533861</v>
+        <v>34065.35250533762</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>7494.377551174495</v>
+        <v>7494.377551174273</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>440.4567379656818</v>
+        <v>440.4567379571263</v>
       </c>
     </row>
     <row r="31">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>4.449057959249304</v>
+        <v>4.44905795916288</v>
       </c>
     </row>
     <row r="33">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>444.9057959249311</v>
+        <v>444.9057959162892</v>
       </c>
     </row>
     <row r="35">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>12544.1909493926</v>
+        <v>12544.19094938395</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>9659.027031032299</v>
+        <v>9659.027031025644</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2124.985946827105</v>
+        <v>2124.985946825642</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>440.4567379656818</v>
+        <v>440.4567379571263</v>
       </c>
     </row>
     <row r="40">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>288923.151613158</v>
+        <v>288923.1516131578</v>
       </c>
     </row>
     <row r="43">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>27418.04182159284</v>
+        <v>27418.04182158377</v>
       </c>
     </row>
     <row r="45">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>15691.08619186042</v>
+        <v>15691.08619185855</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>25152.17161215243</v>
+        <v>25152.17161215057</v>
       </c>
     </row>
     <row r="48">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2265.870209440413</v>
+        <v>2265.870209433193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>